<commit_message>
Restocking of Invetory for regular units
</commit_message>
<xml_diff>
--- a/TestData/InventoryData/InventoryTestCase.xlsx
+++ b/TestData/InventoryData/InventoryTestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\InventoryData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EA17AE-FE42-4974-949A-2B0BB56BB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE82BFAF-C299-4B42-B936-1B8639599306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>frugal@latido.com.np</t>
   </si>
@@ -144,7 +144,52 @@
     <t>quality</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Test01</t>
+  </si>
+  <si>
+    <t>T01</t>
+  </si>
+  <si>
+    <t>Automation Testing Category</t>
+  </si>
+  <si>
+    <t>AT01</t>
+  </si>
+  <si>
+    <t>Auto Testing 01</t>
+  </si>
+  <si>
+    <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\Black Plain Jacket.jpg</t>
+  </si>
+  <si>
+    <t>Pay_mode</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>By Cheque</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\Receipt.png</t>
+  </si>
+  <si>
+    <t>receiver_name</t>
+  </si>
+  <si>
+    <t>2023-05-24</t>
+  </si>
+  <si>
+    <t>transport_mode</t>
+  </si>
+  <si>
+    <t>By Truck</t>
+  </si>
+  <si>
+    <t>ItmeName</t>
   </si>
 </sst>
 </file>
@@ -195,11 +240,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -550,10 +594,13 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="A1:N2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -607,19 +654,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -634,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
         <v>27</v>
@@ -644,6 +691,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{60D2E1E7-0FB9-4F2A-8A4D-332396478053}"/>
   </hyperlinks>
@@ -654,18 +702,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA4ACBA-B1EC-4549-8123-867E1664920E}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="8.88671875" style="3"/>
+    <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -673,25 +721,37 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>38</v>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,13 +759,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2000</v>
       </c>
-      <c r="E2" s="2">
-        <v>45048</v>
+      <c r="F2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Product Management code-base with new features for Duplicating a leather profile
</commit_message>
<xml_diff>
--- a/TestData/InventoryData/InventoryTestCase.xlsx
+++ b/TestData/InventoryData/InventoryTestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\InventoryData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E301F8B-8557-4C18-BD0C-B26669652CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0014FDE1-AE1D-4178-B52A-D844DF77EFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestInventory" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="99">
   <si>
     <t>frugal@latido.com.np</t>
   </si>
@@ -138,9 +138,6 @@
     <t>receiver_name</t>
   </si>
   <si>
-    <t>2023-05-24</t>
-  </si>
-  <si>
     <t>transport_mode</t>
   </si>
   <si>
@@ -165,27 +162,9 @@
     <t>Piece</t>
   </si>
   <si>
-    <t>Leather (Automation)</t>
-  </si>
-  <si>
     <t>This is from an automated Script ( for Leather ) 01</t>
   </si>
   <si>
-    <t>Item 01 (Automation)</t>
-  </si>
-  <si>
-    <t>Item 02 (Automation)</t>
-  </si>
-  <si>
-    <t>Item 03 (Automation)</t>
-  </si>
-  <si>
-    <t>Item 04 (Automation)</t>
-  </si>
-  <si>
-    <t>Item 05 (Automation)</t>
-  </si>
-  <si>
     <t>This is from an automated Script (02)</t>
   </si>
   <si>
@@ -198,9 +177,6 @@
     <t>This is from an automated Script (05)</t>
   </si>
   <si>
-    <t>Auto Testing 06</t>
-  </si>
-  <si>
     <t>AKM Leather</t>
   </si>
   <si>
@@ -213,9 +189,6 @@
     <t>Silver Zipper Supplier</t>
   </si>
   <si>
-    <t>Traders</t>
-  </si>
-  <si>
     <t>Good</t>
   </si>
   <si>
@@ -225,133 +198,133 @@
     <t>By Cash</t>
   </si>
   <si>
-    <t>2023-05-19</t>
-  </si>
-  <si>
-    <t>2023-05-20</t>
-  </si>
-  <si>
-    <t>2023-05-21</t>
-  </si>
-  <si>
-    <t>2023-05-22</t>
-  </si>
-  <si>
-    <t>2023-05-23</t>
-  </si>
-  <si>
     <t>TAT11B</t>
   </si>
   <si>
-    <t>Leather002</t>
-  </si>
-  <si>
-    <t>(Automation) Item 6</t>
-  </si>
-  <si>
-    <t>(Automation) Item 7</t>
-  </si>
-  <si>
-    <t>(Automation) Item 8</t>
-  </si>
-  <si>
-    <t>(Automation) Item 9</t>
-  </si>
-  <si>
-    <t>(Automation) Item 10</t>
-  </si>
-  <si>
-    <t>LT-02</t>
-  </si>
-  <si>
-    <t>AT-IT-6</t>
-  </si>
-  <si>
-    <t>AT-IT-7</t>
-  </si>
-  <si>
-    <t>AT-IT-8</t>
-  </si>
-  <si>
-    <t>AT-IT-9</t>
-  </si>
-  <si>
-    <t>AT-IT-10</t>
-  </si>
-  <si>
     <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\Fraper leather Jacket.jpg</t>
   </si>
   <si>
     <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\David Leather Jacket.jpg</t>
   </si>
   <si>
-    <t>Test07</t>
-  </si>
-  <si>
-    <t>Test08</t>
-  </si>
-  <si>
-    <t>Test09</t>
-  </si>
-  <si>
-    <t>Test10</t>
-  </si>
-  <si>
-    <t>Test11</t>
-  </si>
-  <si>
-    <t>Test12</t>
-  </si>
-  <si>
-    <t>T07</t>
-  </si>
-  <si>
-    <t>T08</t>
-  </si>
-  <si>
-    <t>T09</t>
-  </si>
-  <si>
-    <t>T10</t>
-  </si>
-  <si>
-    <t>T11</t>
-  </si>
-  <si>
-    <t>T12</t>
-  </si>
-  <si>
-    <t>AT07</t>
-  </si>
-  <si>
-    <t>AT08</t>
-  </si>
-  <si>
-    <t>AT09</t>
-  </si>
-  <si>
-    <t>AT10</t>
-  </si>
-  <si>
-    <t>AT11</t>
-  </si>
-  <si>
-    <t>AT12</t>
-  </si>
-  <si>
-    <t>Auto Testing 07</t>
-  </si>
-  <si>
-    <t>Auto Testing 08</t>
-  </si>
-  <si>
-    <t>Auto Testing 09</t>
-  </si>
-  <si>
-    <t>Auto Testing 10</t>
-  </si>
-  <si>
-    <t>Auto Testing 11</t>
+    <t>Leather003</t>
+  </si>
+  <si>
+    <t>(Automation) Item 12</t>
+  </si>
+  <si>
+    <t>(Automation) Item 13</t>
+  </si>
+  <si>
+    <t>Leather001</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\BrowN Leather Beta.png</t>
+  </si>
+  <si>
+    <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\Black Plain Jacket.jpg</t>
+  </si>
+  <si>
+    <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\BikerJacket.jpg</t>
+  </si>
+  <si>
+    <t>2023-06-16</t>
+  </si>
+  <si>
+    <t>Leather00-12</t>
+  </si>
+  <si>
+    <t>LT-012</t>
+  </si>
+  <si>
+    <t>(Automation) Item 65</t>
+  </si>
+  <si>
+    <t>AT-IT-65</t>
+  </si>
+  <si>
+    <t>(Automation) Item 66</t>
+  </si>
+  <si>
+    <t>AT-IT-66</t>
+  </si>
+  <si>
+    <t>(Automation) Item 67</t>
+  </si>
+  <si>
+    <t>AT-IT-67</t>
+  </si>
+  <si>
+    <t>(Automation) Item 68</t>
+  </si>
+  <si>
+    <t>AT-IT-68</t>
+  </si>
+  <si>
+    <t>(Automation) Item 69</t>
+  </si>
+  <si>
+    <t>AT-IT-69</t>
+  </si>
+  <si>
+    <t>T0-LT-00-03</t>
+  </si>
+  <si>
+    <t>AT-LT-00-03</t>
+  </si>
+  <si>
+    <t>T065</t>
+  </si>
+  <si>
+    <t>AT065</t>
+  </si>
+  <si>
+    <t>Auto Testing 65</t>
+  </si>
+  <si>
+    <t>Auto Testing 39</t>
+  </si>
+  <si>
+    <t>T066</t>
+  </si>
+  <si>
+    <t>AT066</t>
+  </si>
+  <si>
+    <t>Auto Testing 66</t>
+  </si>
+  <si>
+    <t>T067</t>
+  </si>
+  <si>
+    <t>AT067</t>
+  </si>
+  <si>
+    <t>Auto Testing 67</t>
+  </si>
+  <si>
+    <t>T068</t>
+  </si>
+  <si>
+    <t>AT068</t>
+  </si>
+  <si>
+    <t>Auto Testing 68</t>
+  </si>
+  <si>
+    <t>T069</t>
+  </si>
+  <si>
+    <t>AT069</t>
+  </si>
+  <si>
+    <t>Auto Testing 69</t>
   </si>
 </sst>
 </file>
@@ -690,7 +663,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="D2" sqref="D2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +688,7 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -729,16 +702,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -752,13 +725,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
         <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -778,22 +751,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -804,22 +777,22 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -830,22 +803,22 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -856,22 +829,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -893,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEFFD9A-D3B2-46BE-B0B0-B1F2C5B65C29}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,19 +927,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -981,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -998,19 +971,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -1025,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
@@ -1045,16 +1018,16 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
         <v>87</v>
       </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -1069,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
@@ -1086,19 +1059,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
@@ -1113,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="M5" t="s">
         <v>23</v>
@@ -1130,19 +1103,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
         <v>95</v>
-      </c>
-      <c r="F6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" t="s">
-        <v>106</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
@@ -1157,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="M6" t="s">
         <v>23</v>
@@ -1174,19 +1147,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -1201,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
         <v>23</v>
@@ -1227,18 +1200,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA4ACBA-B1EC-4549-8123-867E1664920E}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1246,261 +1219,282 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2">
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3">
         <v>2000</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2">
+      <c r="G3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5">
+        <v>2000</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6">
+        <v>2000</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L6" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7">
         <v>2000</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3">
+      <c r="G7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4">
-        <v>2000</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5">
-        <v>2000</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6">
-        <v>2000</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7">
-        <v>2000</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1521,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DFBC77-71EC-407E-ABCC-91907E7A5A93}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1537,7 +1531,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1548,12 +1542,61 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C450EBD3-067F-4159-863E-F570E583D670}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{828313EB-3A58-4C61-A58D-CE2B22D4FD04}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{BC5C2AE9-997F-4334-A362-E1C2B41AE2B2}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{D34E6D1F-E87F-4679-9EA6-DD17F11737ED}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{3C42118C-3376-40A8-90D9-73E1588732FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code base edited with Duplicate Leather data and test file
</commit_message>
<xml_diff>
--- a/TestData/InventoryData/InventoryTestCase.xlsx
+++ b/TestData/InventoryData/InventoryTestCase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\InventoryData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0014FDE1-AE1D-4178-B52A-D844DF77EFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6522AF-C9C4-4695-99D1-68E3FD0EF7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,97 +234,97 @@
     <t>E:\POM_for_Bottle\WebApp\TestData\InventoryData\Image\BikerJacket.jpg</t>
   </si>
   <si>
-    <t>2023-06-16</t>
-  </si>
-  <si>
-    <t>Leather00-12</t>
-  </si>
-  <si>
-    <t>LT-012</t>
-  </si>
-  <si>
-    <t>(Automation) Item 65</t>
-  </si>
-  <si>
-    <t>AT-IT-65</t>
-  </si>
-  <si>
-    <t>(Automation) Item 66</t>
-  </si>
-  <si>
-    <t>AT-IT-66</t>
-  </si>
-  <si>
-    <t>(Automation) Item 67</t>
-  </si>
-  <si>
-    <t>AT-IT-67</t>
-  </si>
-  <si>
-    <t>(Automation) Item 68</t>
-  </si>
-  <si>
-    <t>AT-IT-68</t>
-  </si>
-  <si>
-    <t>(Automation) Item 69</t>
-  </si>
-  <si>
-    <t>AT-IT-69</t>
-  </si>
-  <si>
-    <t>T0-LT-00-03</t>
-  </si>
-  <si>
-    <t>AT-LT-00-03</t>
-  </si>
-  <si>
-    <t>T065</t>
-  </si>
-  <si>
-    <t>AT065</t>
-  </si>
-  <si>
-    <t>Auto Testing 65</t>
-  </si>
-  <si>
-    <t>Auto Testing 39</t>
-  </si>
-  <si>
-    <t>T066</t>
-  </si>
-  <si>
-    <t>AT066</t>
-  </si>
-  <si>
-    <t>Auto Testing 66</t>
-  </si>
-  <si>
-    <t>T067</t>
-  </si>
-  <si>
-    <t>AT067</t>
-  </si>
-  <si>
-    <t>Auto Testing 67</t>
-  </si>
-  <si>
-    <t>T068</t>
-  </si>
-  <si>
-    <t>AT068</t>
-  </si>
-  <si>
-    <t>Auto Testing 68</t>
-  </si>
-  <si>
-    <t>T069</t>
-  </si>
-  <si>
-    <t>AT069</t>
-  </si>
-  <si>
-    <t>Auto Testing 69</t>
+    <t>Leather00-13</t>
+  </si>
+  <si>
+    <t>LT-013</t>
+  </si>
+  <si>
+    <t>(Automation) Item 70</t>
+  </si>
+  <si>
+    <t>AT-IT-70</t>
+  </si>
+  <si>
+    <t>(Automation) Item 71</t>
+  </si>
+  <si>
+    <t>AT-IT-71</t>
+  </si>
+  <si>
+    <t>(Automation) Item 72</t>
+  </si>
+  <si>
+    <t>AT-IT-72</t>
+  </si>
+  <si>
+    <t>(Automation) Item 73</t>
+  </si>
+  <si>
+    <t>AT-IT-73</t>
+  </si>
+  <si>
+    <t>(Automation) Item 74</t>
+  </si>
+  <si>
+    <t>AT-IT-74</t>
+  </si>
+  <si>
+    <t>T0-LT-00-04</t>
+  </si>
+  <si>
+    <t>AT-LT-00-04</t>
+  </si>
+  <si>
+    <t>T070</t>
+  </si>
+  <si>
+    <t>AT070</t>
+  </si>
+  <si>
+    <t>T071</t>
+  </si>
+  <si>
+    <t>AT071</t>
+  </si>
+  <si>
+    <t>T072</t>
+  </si>
+  <si>
+    <t>AT072</t>
+  </si>
+  <si>
+    <t>T073</t>
+  </si>
+  <si>
+    <t>AT073</t>
+  </si>
+  <si>
+    <t>T074</t>
+  </si>
+  <si>
+    <t>AT074</t>
+  </si>
+  <si>
+    <t>Auto Testing -004</t>
+  </si>
+  <si>
+    <t>Auto Testing 70</t>
+  </si>
+  <si>
+    <t>Auto Testing 71</t>
+  </si>
+  <si>
+    <t>Auto Testing 72</t>
+  </si>
+  <si>
+    <t>Auto Testing 73</t>
+  </si>
+  <si>
+    <t>Auto Testing 74</t>
+  </si>
+  <si>
+    <t>2023-07-07</t>
   </si>
 </sst>
 </file>
@@ -705,10 +705,10 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -728,10 +728,10 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
         <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -754,10 +754,10 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" t="s">
-        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>45</v>
@@ -780,10 +780,10 @@
         <v>67</v>
       </c>
       <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
         <v>75</v>
-      </c>
-      <c r="E5" t="s">
-        <v>76</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>
@@ -806,10 +806,10 @@
         <v>66</v>
       </c>
       <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
         <v>77</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -832,10 +832,10 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
         <v>79</v>
-      </c>
-      <c r="E7" t="s">
-        <v>80</v>
       </c>
       <c r="F7" t="s">
         <v>48</v>
@@ -867,7 +867,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,19 +927,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
       <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
         <v>81</v>
       </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -971,19 +971,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
       <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
         <v>83</v>
       </c>
-      <c r="F3" t="s">
-        <v>84</v>
-      </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -1015,19 +1015,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -1059,19 +1059,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
@@ -1103,19 +1103,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
         <v>77</v>
       </c>
-      <c r="D6" t="s">
-        <v>78</v>
-      </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
@@ -1147,19 +1147,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="D7" t="s">
-        <v>80</v>
-      </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" t="s">
         <v>97</v>
-      </c>
-      <c r="G7" t="s">
-        <v>98</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C2" sqref="C2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,10 +1260,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
@@ -1272,7 +1272,7 @@
         <v>2000</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -1301,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -1313,7 +1313,7 @@
         <v>2000</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -1342,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -1354,7 +1354,7 @@
         <v>2000</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -1383,10 +1383,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>76</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -1395,7 +1395,7 @@
         <v>2000</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -1424,10 +1424,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -1436,7 +1436,7 @@
         <v>2000</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -1465,10 +1465,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
         <v>79</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>63</v>
@@ -1477,7 +1477,7 @@
         <v>2000</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H7">
         <v>10</v>

</xml_diff>

<commit_message>
Added Product Management, Leather Management,Product Category, Blog
</commit_message>
<xml_diff>
--- a/TestData/InventoryData/InventoryTestCase.xlsx
+++ b/TestData/InventoryData/InventoryTestCase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\InventoryData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291DE758-9D7A-4503-B516-0CE285F9DF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D548F5D3-BCCB-4FCA-A381-A137FBF11E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
   <si>
     <t>frugal@latido.com.np</t>
   </si>
@@ -234,94 +234,106 @@
     <t>2023-07-07</t>
   </si>
   <si>
-    <t>Leather00-18</t>
-  </si>
-  <si>
-    <t>LT-018</t>
-  </si>
-  <si>
-    <t>(Automation) Item 90</t>
-  </si>
-  <si>
-    <t>AT-IT-90</t>
-  </si>
-  <si>
-    <t>(Automation) Item 91</t>
-  </si>
-  <si>
-    <t>AT-IT-91</t>
-  </si>
-  <si>
-    <t>(Automation) Item 92</t>
-  </si>
-  <si>
-    <t>AT-IT-92</t>
-  </si>
-  <si>
-    <t>(Automation) Item 93</t>
-  </si>
-  <si>
-    <t>AT-IT-93</t>
-  </si>
-  <si>
-    <t>(Automation) Item 94</t>
-  </si>
-  <si>
-    <t>AT-IT-94</t>
-  </si>
-  <si>
-    <t>T0-LT-00-08</t>
-  </si>
-  <si>
-    <t>AT-LT-00-08</t>
-  </si>
-  <si>
-    <t>Auto Testing -008</t>
-  </si>
-  <si>
-    <t>T090</t>
-  </si>
-  <si>
-    <t>AT090</t>
-  </si>
-  <si>
-    <t>Auto Testing 90</t>
-  </si>
-  <si>
-    <t>T091</t>
-  </si>
-  <si>
-    <t>AT091</t>
-  </si>
-  <si>
-    <t>Auto Testing 91</t>
-  </si>
-  <si>
-    <t>T092</t>
-  </si>
-  <si>
-    <t>AT092</t>
-  </si>
-  <si>
-    <t>Auto Testing 92</t>
-  </si>
-  <si>
-    <t>T093</t>
-  </si>
-  <si>
-    <t>AT093</t>
-  </si>
-  <si>
-    <t>Auto Testing 93</t>
-  </si>
-  <si>
-    <t>T094</t>
-  </si>
-  <si>
-    <t>AT094</t>
-  </si>
-  <si>
-    <t>Auto Testing 94</t>
+    <t>leather_flg</t>
+  </si>
+  <si>
+    <t>leather_ball_imgPath</t>
+  </si>
+  <si>
+    <t>Auto Testing -013</t>
+  </si>
+  <si>
+    <t>Leather00-24</t>
+  </si>
+  <si>
+    <t>LT-024</t>
+  </si>
+  <si>
+    <t>LT-025</t>
+  </si>
+  <si>
+    <t>(Automation) Item 120</t>
+  </si>
+  <si>
+    <t>AT-IT-120</t>
+  </si>
+  <si>
+    <t>(Automation) Item 121</t>
+  </si>
+  <si>
+    <t>AT-IT-121</t>
+  </si>
+  <si>
+    <t>(Automation) Item 122</t>
+  </si>
+  <si>
+    <t>AT-IT-122</t>
+  </si>
+  <si>
+    <t>(Automation) Item 123</t>
+  </si>
+  <si>
+    <t>AT-IT-123</t>
+  </si>
+  <si>
+    <t>(Automation) Item 124</t>
+  </si>
+  <si>
+    <t>AT-IT-124</t>
+  </si>
+  <si>
+    <t>T0-LT-00-24</t>
+  </si>
+  <si>
+    <t>AT-LT-00-24</t>
+  </si>
+  <si>
+    <t>T0120</t>
+  </si>
+  <si>
+    <t>AT0120</t>
+  </si>
+  <si>
+    <t>Auto Testing 120</t>
+  </si>
+  <si>
+    <t>T0121</t>
+  </si>
+  <si>
+    <t>AT0121</t>
+  </si>
+  <si>
+    <t>Auto Testing 121</t>
+  </si>
+  <si>
+    <t>T0122</t>
+  </si>
+  <si>
+    <t>AT0122</t>
+  </si>
+  <si>
+    <t>Auto Testing 122</t>
+  </si>
+  <si>
+    <t>T0123</t>
+  </si>
+  <si>
+    <t>AT0123</t>
+  </si>
+  <si>
+    <t>Auto Testing 123</t>
+  </si>
+  <si>
+    <t>T0124</t>
+  </si>
+  <si>
+    <t>AT0124</t>
+  </si>
+  <si>
+    <t>Auto Testing 124</t>
+  </si>
+  <si>
+    <t>Leather00-25</t>
   </si>
 </sst>
 </file>
@@ -660,7 +672,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E7"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,10 +714,10 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -725,10 +737,10 @@
         <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -751,10 +763,10 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
         <v>45</v>
@@ -777,10 +789,10 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>
@@ -803,10 +815,10 @@
         <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -829,10 +841,10 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
         <v>48</v>
@@ -861,10 +873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEFFD9A-D3B2-46BE-B0B0-B1F2C5B65C29}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D7"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,7 +884,7 @@
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -907,16 +919,22 @@
         <v>17</v>
       </c>
       <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,19 +942,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -950,17 +968,23 @@
       <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>58</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,19 +992,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -994,17 +1018,20 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>66</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1012,19 +1039,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -1038,17 +1065,20 @@
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>58</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>23</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,19 +1086,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
@@ -1082,17 +1112,20 @@
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>57</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>23</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1100,19 +1133,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
@@ -1126,17 +1159,20 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>58</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>23</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,19 +1180,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -1170,13 +1206,16 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>64</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>23</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>50</v>
       </c>
     </row>
@@ -1200,7 +1239,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,10 +1296,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
@@ -1298,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -1339,10 +1378,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -1380,10 +1419,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -1421,10 +1460,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -1462,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>51</v>
@@ -1515,7 +1554,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>